<commit_message>
add some more features
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E468A1D7-921A-47E0-93EA-6EA39719F3A3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B159F9F-DD13-45E6-99C1-C434142F238D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$101</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="177">
   <si>
     <t>字段名称</t>
   </si>
@@ -365,6 +368,192 @@
   </si>
   <si>
     <t>indicate whether ip_prov is same as cert_prov</t>
+  </si>
+  <si>
+    <t>transaction_hour</t>
+  </si>
+  <si>
+    <t>hour of transaction</t>
+  </si>
+  <si>
+    <t>diff_hour</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>avg_prev_amt</t>
+  </si>
+  <si>
+    <t>std_prev_amt</t>
+  </si>
+  <si>
+    <t>ip_prov_vs_prev</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>…………</t>
+  </si>
+  <si>
+    <t>num_prev_ip_prov</t>
+  </si>
+  <si>
+    <t>ip_prov_ratio_among_prev</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>number of hours have passed since last transaction of this user</t>
+  </si>
+  <si>
+    <t>average of previous transaction amounts of this user</t>
+  </si>
+  <si>
+    <t>standard deviation of previous transaction amounts of this user</t>
+  </si>
+  <si>
+    <t>indicate whether the ip_prov of current transaction is same as previous transaction of this user</t>
+  </si>
+  <si>
+    <t>indicate the percentage of current transaction ip_prov among all transaction ip_prov of this user (e.g. 0.4, 0.5, 0.97)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric (0~1), -1 indicating NA </t>
+  </si>
+  <si>
+    <t>-1,0,1 (-1 indicating NA)</t>
+  </si>
+  <si>
+    <t>indicate the number of distinct previously occurred ip_prov</t>
+  </si>
+  <si>
+    <t>numeric (-1 indicating NA)</t>
+  </si>
+  <si>
+    <t>min_prev_amt</t>
+  </si>
+  <si>
+    <t>max_prev_amt</t>
+  </si>
+  <si>
+    <t>maximum of previous transaction amounts of this user</t>
+  </si>
+  <si>
+    <t>minimum of previous transaction amounts of this user</t>
+  </si>
+  <si>
+    <t>transaction_dow</t>
+  </si>
+  <si>
+    <t>transaction day of week</t>
+  </si>
+  <si>
+    <t>transaction_dom</t>
+  </si>
+  <si>
+    <t>transaction day of month</t>
+  </si>
+  <si>
+    <t>diff_day</t>
+  </si>
+  <si>
+    <t>number of days haved passed since last transaction of this user</t>
+  </si>
+  <si>
+    <t>cert_prov_vs_prev</t>
+  </si>
+  <si>
+    <t>card_bin_prov_vs_prev</t>
+  </si>
+  <si>
+    <t>card_mobile_prov_vs_prev</t>
+  </si>
+  <si>
+    <t>card_cert_prov_vs_prev</t>
+  </si>
+  <si>
+    <t>province_vs_prev</t>
+  </si>
+  <si>
+    <t>ip_city_vs_prev</t>
+  </si>
+  <si>
+    <t>cert_city_vs_prev</t>
+  </si>
+  <si>
+    <t>card_bin_city_vs_prev</t>
+  </si>
+  <si>
+    <t>card_mobile_city_vs_prev</t>
+  </si>
+  <si>
+    <t>card_cert_city_vs_prev</t>
+  </si>
+  <si>
+    <t>city_vs_prev</t>
+  </si>
+  <si>
+    <t>client_ip_vs_prev</t>
+  </si>
+  <si>
+    <t>network_vs_prev</t>
+  </si>
+  <si>
+    <t>device_sign_vs_prev</t>
+  </si>
+  <si>
+    <t>info_1_vs_prev</t>
+  </si>
+  <si>
+    <t>info_2_vs_prev</t>
+  </si>
+  <si>
+    <t>is_one_people_vs_prev</t>
+  </si>
+  <si>
+    <t>mobile_oper_platform_vs_prev</t>
+  </si>
+  <si>
+    <t>operation_channel_vs_prev</t>
+  </si>
+  <si>
+    <t>pay_scene_vs_prev</t>
+  </si>
+  <si>
+    <t>card_cert_no_vs_prev</t>
+  </si>
+  <si>
+    <t>opposing_id_vs_prev</t>
+  </si>
+  <si>
+    <t>income_card_no_vs_prev</t>
+  </si>
+  <si>
+    <t>income_card_cert_no_vs_prev</t>
+  </si>
+  <si>
+    <t>income_card_mobile_vs_prev</t>
+  </si>
+  <si>
+    <t>income_card_bank_code_vs_prev</t>
+  </si>
+  <si>
+    <t>is_peer_pay_vs_prev</t>
+  </si>
+  <si>
+    <t>version_vs_prev</t>
+  </si>
+  <si>
+    <t>Done (training)</t>
+  </si>
+  <si>
+    <t>Done (test)</t>
   </si>
 </sst>
 </file>
@@ -414,7 +603,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,6 +640,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,7 +707,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -524,6 +731,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -809,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,9 +1041,11 @@
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
     <col min="3" max="3" width="119.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,16 +1058,28 @@
       <c r="D1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -855,8 +1089,14 @@
       <c r="D3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -866,8 +1106,14 @@
       <c r="D4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -877,8 +1123,14 @@
       <c r="D5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -891,8 +1143,14 @@
       <c r="D6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -902,8 +1160,14 @@
       <c r="D7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -916,8 +1180,14 @@
       <c r="D8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -930,8 +1200,14 @@
       <c r="D9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -941,8 +1217,14 @@
       <c r="D10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -952,8 +1234,14 @@
       <c r="D11" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -963,8 +1251,14 @@
       <c r="D12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -974,8 +1268,14 @@
       <c r="D13" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -988,8 +1288,14 @@
       <c r="D14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1002,8 +1308,14 @@
       <c r="D15" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1013,8 +1325,14 @@
       <c r="D16" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1024,8 +1342,14 @@
       <c r="D17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1038,8 +1362,14 @@
       <c r="D18" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1052,8 +1382,14 @@
       <c r="D19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1066,8 +1402,14 @@
       <c r="D20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1077,8 +1419,14 @@
       <c r="D21" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1088,8 +1436,14 @@
       <c r="D22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1099,8 +1453,14 @@
       <c r="D23" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1110,8 +1470,14 @@
       <c r="D24" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1121,8 +1487,14 @@
       <c r="D25" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -1132,8 +1504,14 @@
       <c r="D26" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -1143,8 +1521,14 @@
       <c r="D27" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -1154,8 +1538,14 @@
       <c r="D28" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -1165,8 +1555,14 @@
       <c r="D29" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -1176,8 +1572,14 @@
       <c r="D30" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1187,8 +1589,14 @@
       <c r="D31" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -1198,8 +1606,14 @@
       <c r="D32" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -1209,8 +1623,14 @@
       <c r="D33" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -1220,8 +1640,14 @@
       <c r="D34" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -1231,161 +1657,1068 @@
       <c r="D35" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E41" t="s">
+        <v>126</v>
+      </c>
+      <c r="F41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" t="s">
+        <v>126</v>
+      </c>
+      <c r="F42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" t="s">
+        <v>126</v>
+      </c>
+      <c r="F43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E45" t="s">
+        <v>126</v>
+      </c>
+      <c r="F45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" t="s">
+        <v>126</v>
+      </c>
+      <c r="F46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D48" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D49" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E49" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D50" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" t="s">
+        <v>126</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D51" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D52" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E52" t="s">
+        <v>126</v>
+      </c>
+      <c r="F52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D53" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E53" t="s">
+        <v>126</v>
+      </c>
+      <c r="F53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D54" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E54" t="s">
+        <v>126</v>
+      </c>
+      <c r="F54" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D55" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E55" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D56" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" t="s">
+        <v>126</v>
+      </c>
+      <c r="F56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D57" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" t="s">
+        <v>126</v>
+      </c>
+      <c r="F57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D58" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" t="s">
+        <v>126</v>
+      </c>
+      <c r="F58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D59" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E59" t="s">
+        <v>126</v>
+      </c>
+      <c r="F59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D60" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E60" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D61" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E61" t="s">
+        <v>126</v>
+      </c>
+      <c r="F61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D62" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D63" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" t="s">
+        <v>126</v>
+      </c>
+      <c r="F63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D64" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E64" t="s">
+        <v>126</v>
+      </c>
+      <c r="F64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>113</v>
       </c>
+      <c r="D65" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D66" t="s">
+        <v>118</v>
+      </c>
+      <c r="E66" t="s">
+        <v>126</v>
+      </c>
+      <c r="F66" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" t="s">
+        <v>126</v>
+      </c>
+      <c r="F67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" t="s">
+        <v>144</v>
+      </c>
+      <c r="D68" t="s">
+        <v>118</v>
+      </c>
+      <c r="E68" t="s">
+        <v>126</v>
+      </c>
+      <c r="F68" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" t="s">
+        <v>128</v>
+      </c>
+      <c r="D69" t="s">
+        <v>118</v>
+      </c>
+      <c r="E69" t="s">
+        <v>126</v>
+      </c>
+      <c r="F69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70" t="s">
+        <v>146</v>
+      </c>
+      <c r="D70" t="s">
+        <v>118</v>
+      </c>
+      <c r="E70" t="s">
+        <v>126</v>
+      </c>
+      <c r="F70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" t="s">
+        <v>131</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E71" t="s">
+        <v>126</v>
+      </c>
+      <c r="F71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E72" t="s">
+        <v>126</v>
+      </c>
+      <c r="F72" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E73" t="s">
+        <v>126</v>
+      </c>
+      <c r="F73" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E74" t="s">
+        <v>126</v>
+      </c>
+      <c r="F74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" t="s">
+        <v>126</v>
+      </c>
+      <c r="F75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E76" t="s">
+        <v>126</v>
+      </c>
+      <c r="F76" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E77" t="s">
+        <v>126</v>
+      </c>
+      <c r="F77" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" t="s">
+        <v>126</v>
+      </c>
+      <c r="F78" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E79" t="s">
+        <v>126</v>
+      </c>
+      <c r="F79" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E80" t="s">
+        <v>126</v>
+      </c>
+      <c r="F80" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" t="s">
+        <v>126</v>
+      </c>
+      <c r="F81" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E82" t="s">
+        <v>126</v>
+      </c>
+      <c r="F82" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E83" t="s">
+        <v>126</v>
+      </c>
+      <c r="F83" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E84" t="s">
+        <v>126</v>
+      </c>
+      <c r="F84" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E85" t="s">
+        <v>126</v>
+      </c>
+      <c r="F85" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E86" t="s">
+        <v>126</v>
+      </c>
+      <c r="F86" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E87" t="s">
+        <v>126</v>
+      </c>
+      <c r="F87" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E88" t="s">
+        <v>126</v>
+      </c>
+      <c r="F88" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E89" t="s">
+        <v>126</v>
+      </c>
+      <c r="F89" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E90" t="s">
+        <v>126</v>
+      </c>
+      <c r="F90" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E91" t="s">
+        <v>126</v>
+      </c>
+      <c r="F91" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E92" t="s">
+        <v>126</v>
+      </c>
+      <c r="F92" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E93" t="s">
+        <v>126</v>
+      </c>
+      <c r="F93" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E94" t="s">
+        <v>126</v>
+      </c>
+      <c r="F94" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E95" t="s">
+        <v>126</v>
+      </c>
+      <c r="F95" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E96" t="s">
+        <v>126</v>
+      </c>
+      <c r="F96" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E97" t="s">
+        <v>126</v>
+      </c>
+      <c r="F97" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E98" t="s">
+        <v>126</v>
+      </c>
+      <c r="F98" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E99" t="s">
+        <v>126</v>
+      </c>
+      <c r="F99" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C100" t="s">
+        <v>129</v>
+      </c>
+      <c r="D100" t="s">
+        <v>136</v>
+      </c>
+      <c r="E100" t="s">
+        <v>126</v>
+      </c>
+      <c r="F100" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C101" t="s">
+        <v>130</v>
+      </c>
+      <c r="D101" t="s">
+        <v>136</v>
+      </c>
+      <c r="E101" t="s">
+        <v>126</v>
+      </c>
+      <c r="F101" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C102" t="s">
+        <v>139</v>
+      </c>
+      <c r="D102" t="s">
+        <v>136</v>
+      </c>
+      <c r="E102" t="s">
+        <v>126</v>
+      </c>
+      <c r="F102" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C103" t="s">
+        <v>140</v>
+      </c>
+      <c r="D103" t="s">
+        <v>136</v>
+      </c>
+      <c r="E103" t="s">
+        <v>126</v>
+      </c>
+      <c r="F103" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C104" t="s">
+        <v>135</v>
+      </c>
+      <c r="D104" t="s">
+        <v>136</v>
+      </c>
+      <c r="E104" t="s">
+        <v>127</v>
+      </c>
+      <c r="F104" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C105" t="s">
+        <v>123</v>
+      </c>
+      <c r="D105" t="s">
+        <v>136</v>
+      </c>
+      <c r="E105" t="s">
+        <v>127</v>
+      </c>
+      <c r="F105" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C106" t="s">
+        <v>132</v>
+      </c>
+      <c r="D106" t="s">
+        <v>133</v>
+      </c>
+      <c r="E106" t="s">
+        <v>127</v>
+      </c>
+      <c r="F106" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C107" t="s">
+        <v>123</v>
+      </c>
+      <c r="D107" t="s">
+        <v>133</v>
+      </c>
+      <c r="E107" t="s">
+        <v>127</v>
+      </c>
+      <c r="F107" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D72" xr:uid="{076E19BD-AA5B-475C-9E41-86F5F43468AD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>